<commit_message>
Complete The Project Simple Functionality
</commit_message>
<xml_diff>
--- a/TicTacToeGame/Task.xlsx
+++ b/TicTacToeGame/Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Udemy\NAM.NET-repos\TicTacToeGame\TicTacToeGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{300023DC-E1D8-4FC0-9396-4CE0C69390D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4B3739-385D-40B2-98F2-2D641C927C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{57B84F26-D003-4280-A229-6755C1DF39B5}"/>
   </bookViews>
@@ -188,6 +188,24 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -200,24 +218,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -243,12 +243,12 @@
   <autoFilter ref="A1:E22" xr:uid="{D875DDCF-65A8-4055-99B7-F0C40C99862D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EE02B2AD-4BE3-4567-A3E1-860804FF86AE}" name="Number" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{8FACBCE6-7B8D-4679-9445-F2384BDE1344}" name="Task" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{61A9C9F4-EE1A-4956-A3A2-6A434A452529}" name="Task Type" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{8FACBCE6-7B8D-4679-9445-F2384BDE1344}" name="Task" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{61A9C9F4-EE1A-4956-A3A2-6A434A452529}" name="Task Type" dataDxfId="8">
       <calculatedColumnFormula>$H$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8239D9DB-FE4E-4A57-8743-072B014DE2DC}" name="Solution" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{DFBA1661-F9FD-4F09-A381-A0A16810B36F}" name="Status" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{8239D9DB-FE4E-4A57-8743-072B014DE2DC}" name="Solution" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DFBA1661-F9FD-4F09-A381-A0A16810B36F}" name="Status" dataDxfId="6">
       <calculatedColumnFormula>$G$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -257,20 +257,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A326684-F8A3-4986-A6BA-547F9AF62E1D}" name="Table2" displayName="Table2" ref="G1:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A326684-F8A3-4986-A6BA-547F9AF62E1D}" name="Table2" displayName="Table2" ref="G1:G5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="G1:G5" xr:uid="{8A326684-F8A3-4986-A6BA-547F9AF62E1D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{16649130-B532-4189-84F6-DF71AF1FC3E8}" name="Status Type" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{16649130-B532-4189-84F6-DF71AF1FC3E8}" name="Status Type" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7EB57B95-790F-406D-B9FE-5AA47A924278}" name="Table24" displayName="Table24" ref="H1:H5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7EB57B95-790F-406D-B9FE-5AA47A924278}" name="Table24" displayName="Table24" ref="H1:H5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="H1:H5" xr:uid="{7EB57B95-790F-406D-B9FE-5AA47A924278}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2CE0ADC0-78EB-452E-8D05-2BC3D36DDC1B}" name="Task Type" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{2CE0ADC0-78EB-452E-8D05-2BC3D36DDC1B}" name="Task Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061F245B-933F-4894-A43C-3A8DDBE7E637}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,15 +642,15 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C22" si="0">$H$3</f>
+        <f t="shared" ref="C2:C9" si="0">$H$3</f>
         <v>Backend</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>$G$3</f>
-        <v>In Progress</v>
+        <f>$G$4</f>
+        <v>Done</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -699,7 +699,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f t="shared" ref="E4:E22" si="1">$G$2</f>
+        <f t="shared" ref="E4:E13" si="1">$G$2</f>
         <v>Open</v>
       </c>
       <c r="G4" s="3" t="s">

</xml_diff>